<commit_message>
add location extraction from XLS
</commit_message>
<xml_diff>
--- a/resources/gameBook.xlsx
+++ b/resources/gameBook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhhongxi/Desktop/LoversQuest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F052884-7926-B642-9163-38EEFD7A4FB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A0B3940-054A-1142-8E05-06BAA5CD38A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20420" xr2:uid="{441C05F4-22D2-7348-A0BD-AC64BB4D47F4}"/>
+    <workbookView xWindow="38400" yWindow="460" windowWidth="35840" windowHeight="19620" xr2:uid="{441C05F4-22D2-7348-A0BD-AC64BB4D47F4}"/>
   </bookViews>
   <sheets>
     <sheet name="location" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="106">
   <si>
     <t xml:space="preserve">Name </t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>Drill SGT Spitting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Barracks </t>
   </si>
   <si>
     <t>PX</t>
@@ -725,7 +722,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -739,16 +736,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
@@ -756,154 +753,154 @@
     </row>
     <row r="2" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>105</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -927,136 +924,136 @@
   <sheetData>
     <row r="1" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>88</v>
       </c>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>90</v>
       </c>
       <c r="C15" s="2"/>
     </row>
@@ -1081,50 +1078,50 @@
   <sheetData>
     <row r="1" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1149,7 +1146,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1158,147 +1155,147 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
         <v>41</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>42</v>
       </c>
-      <c r="C11" t="s">
-        <v>43</v>
-      </c>
       <c r="D11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add NPC to map
</commit_message>
<xml_diff>
--- a/resources/gameBook.xlsx
+++ b/resources/gameBook.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhhongxi/Desktop/LoversQuest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A0B3940-054A-1142-8E05-06BAA5CD38A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D10B46-46D2-514C-9139-843F9CF8536E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="460" windowWidth="35840" windowHeight="19620" xr2:uid="{441C05F4-22D2-7348-A0BD-AC64BB4D47F4}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20420" activeTab="3" xr2:uid="{441C05F4-22D2-7348-A0BD-AC64BB4D47F4}"/>
   </bookViews>
   <sheets>
     <sheet name="location" sheetId="1" r:id="rId1"/>
     <sheet name="item" sheetId="3" r:id="rId2"/>
     <sheet name="container" sheetId="4" r:id="rId3"/>
-    <sheet name="npc" sheetId="2" r:id="rId4"/>
+    <sheet name="npc" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -114,9 +114,6 @@
     <t>Drill_PT</t>
   </si>
   <si>
-    <t>Drill_LandNav</t>
-  </si>
-  <si>
     <t>Drill_Range</t>
   </si>
   <si>
@@ -352,6 +349,9 @@
   </si>
   <si>
     <t>Barracks</t>
+  </si>
+  <si>
+    <t>Drill_CLS</t>
   </si>
 </sst>
 </file>
@@ -401,10 +401,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -721,7 +722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C858C57-114F-F547-B796-5E0DB4646590}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -736,16 +737,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
@@ -765,7 +766,7 @@
     </row>
     <row r="3" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
@@ -803,7 +804,7 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>15</v>
@@ -820,7 +821,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -839,7 +840,7 @@
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>12</v>
@@ -924,136 +925,136 @@
   <sheetData>
     <row r="1" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="C15" s="2"/>
     </row>
@@ -1078,50 +1079,50 @@
   <sheetData>
     <row r="1" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1130,172 +1131,174 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8F03C60-A5E6-0E49-A85D-9692C498EA4D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF017B32-F13C-9940-ADCC-028F3D0515B4}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
-    <col min="3" max="3" width="67.5" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="3"/>
+    <col min="2" max="2" width="62.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="3"/>
+    <col min="4" max="4" width="21.33203125" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="D2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="D3" t="s">
         <v>24</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B5" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="D6" t="s">
         <v>26</v>
       </c>
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="D9" t="s">
         <v>29</v>
       </c>
-      <c r="B8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" t="s">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="D10" t="s">
         <v>30</v>
       </c>
-      <c r="B9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" t="s">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" t="s">
         <v>39</v>
-      </c>
-      <c r="C10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add item, container, npc to front end
</commit_message>
<xml_diff>
--- a/resources/gameBook.xlsx
+++ b/resources/gameBook.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhhongxi/Desktop/LoversQuest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D10B46-46D2-514C-9139-843F9CF8536E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B7A525-F49B-3241-A070-259C2096343B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20420" activeTab="3" xr2:uid="{441C05F4-22D2-7348-A0BD-AC64BB4D47F4}"/>
   </bookViews>
   <sheets>
     <sheet name="location" sheetId="1" r:id="rId1"/>
     <sheet name="item" sheetId="3" r:id="rId2"/>
-    <sheet name="container" sheetId="4" r:id="rId3"/>
+    <sheet name="container" sheetId="6" r:id="rId3"/>
     <sheet name="npc" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="115">
   <si>
     <t xml:space="preserve">Name </t>
   </si>
@@ -135,9 +135,6 @@
     <t>Drill SGT Dicks</t>
   </si>
   <si>
-    <t>Drill SGT Nogo</t>
-  </si>
-  <si>
     <t>Drill SGT Hawkeyes</t>
   </si>
   <si>
@@ -168,9 +165,6 @@
     <t xml:space="preserve">is looking for </t>
   </si>
   <si>
-    <t xml:space="preserve">is mark off </t>
-  </si>
-  <si>
     <t xml:space="preserve">is fixing </t>
   </si>
   <si>
@@ -309,15 +303,9 @@
     <t>Ammo Box</t>
   </si>
   <si>
-    <t>Full of brass and whiteclaws</t>
-  </si>
-  <si>
     <t>Trash Can</t>
   </si>
   <si>
-    <t>Just your hopes and dreams</t>
-  </si>
-  <si>
     <t>IFAK</t>
   </si>
   <si>
@@ -327,15 +315,9 @@
     <t>Ceiling Tile</t>
   </si>
   <si>
-    <t>It's dusty up here</t>
-  </si>
-  <si>
     <t>Foot Locker</t>
   </si>
   <si>
-    <t xml:space="preserve">your personal safe place </t>
-  </si>
-  <si>
     <t>EAST</t>
   </si>
   <si>
@@ -352,6 +334,51 @@
   </si>
   <si>
     <t>Drill_CLS</t>
+  </si>
+  <si>
+    <t>Miliatry Clothing &amp; Class 5</t>
+  </si>
+  <si>
+    <t>Natural Lime WhiteClaw,Ruby Grapefruit WhiteClaw,Black Cherry WhiteClaw</t>
+  </si>
+  <si>
+    <t>M16 Assault Rifle, CamelBack,Sick call slip</t>
+  </si>
+  <si>
+    <t>Natural Lime WhiteClaw,Ruby Grapefruit WhiteClaw,Black Cherry WhiteClaw,Mango WhiteClaw,Diamond Ring</t>
+  </si>
+  <si>
+    <t>ItemInContainer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Location </t>
+  </si>
+  <si>
+    <t>laundry room</t>
+  </si>
+  <si>
+    <t>Sick Call Slip</t>
+  </si>
+  <si>
+    <t>contain full of brass and whiteclaws</t>
+  </si>
+  <si>
+    <t>just full of your hopes and dreams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to be your personal safe place </t>
+  </si>
+  <si>
+    <t>is a place always rips you off</t>
+  </si>
+  <si>
+    <t>is a perfect place to hide contrabands</t>
+  </si>
+  <si>
+    <t>Drill SGT Tourniquette</t>
+  </si>
+  <si>
+    <t>is CLS instructor and will add game interface here</t>
   </si>
 </sst>
 </file>
@@ -737,16 +764,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
@@ -766,7 +793,7 @@
     </row>
     <row r="3" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
@@ -804,7 +831,7 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>15</v>
@@ -821,7 +848,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -840,7 +867,7 @@
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>12</v>
@@ -914,147 +941,147 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="A2" sqref="A2:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="1" max="1" width="46.33203125" customWidth="1"/>
     <col min="2" max="2" width="38.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C15" s="2"/>
     </row>
@@ -1064,65 +1091,114 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E64E0687-E957-D34F-A426-1F77844B1C49}">
-  <dimension ref="A1:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10AEA802-0E88-B24C-A9B4-36B13C3531BC}">
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="55.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="62.5" customWidth="1"/>
+    <col min="3" max="3" width="96.1640625" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B3" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="C4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B5" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>98</v>
-      </c>
       <c r="B6" s="2" t="s">
-        <v>99</v>
+        <v>110</v>
+      </c>
+      <c r="C6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1135,12 +1211,12 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="3"/>
+    <col min="1" max="1" width="27.1640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="62.33203125" style="3" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="3"/>
     <col min="4" max="4" width="21.33203125" style="3" customWidth="1"/>
@@ -1155,7 +1231,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D1" t="s">
         <v>22</v>
@@ -1166,10 +1242,10 @@
         <v>31</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="D2" t="s">
         <v>23</v>
@@ -1180,10 +1256,10 @@
         <v>32</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D3" t="s">
         <v>24</v>
@@ -1194,10 +1270,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
         <v>25</v>
@@ -1205,27 +1281,27 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>33</v>
+        <v>113</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>44</v>
+        <v>114</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
         <v>26</v>
@@ -1233,13 +1309,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D7" t="s">
         <v>27</v>
@@ -1247,13 +1323,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D8" t="s">
         <v>28</v>
@@ -1261,13 +1337,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D9" t="s">
         <v>29</v>
@@ -1275,13 +1351,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D10" t="s">
         <v>30</v>
@@ -1289,16 +1365,16 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="C11" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit before merge david's clsgame
</commit_message>
<xml_diff>
--- a/resources/gameBook.xlsx
+++ b/resources/gameBook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhhongxi/Desktop/LoversQuest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1711DE7E-A0F3-4B4A-8221-85B36BF1882A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7212A80D-30AE-D942-9069-11D60EB637FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38380" yWindow="460" windowWidth="35840" windowHeight="20420" activeTab="3" xr2:uid="{441C05F4-22D2-7348-A0BD-AC64BB4D47F4}"/>
+    <workbookView xWindow="38380" yWindow="460" windowWidth="35840" windowHeight="20420" xr2:uid="{441C05F4-22D2-7348-A0BD-AC64BB4D47F4}"/>
   </bookViews>
   <sheets>
     <sheet name="objInGame" sheetId="7" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="128">
   <si>
     <t xml:space="preserve">Name </t>
   </si>
@@ -413,6 +413,12 @@
   </si>
   <si>
     <t>Natural Lime White Claw,Ruby Grapefruit White Claw,Black Cherry White Claw</t>
+  </si>
+  <si>
+    <t>play</t>
+  </si>
+  <si>
+    <t>game</t>
   </si>
 </sst>
 </file>
@@ -781,10 +787,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51334EF7-C71C-3B45-98D3-0385A5E3D9BA}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -796,7 +802,7 @@
     <col min="5" max="5" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>119</v>
       </c>
@@ -815,8 +821,11 @@
       <c r="F1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>31</v>
       </c>
@@ -835,8 +844,11 @@
       <c r="F2" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>32</v>
       </c>
@@ -853,7 +865,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -870,7 +882,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>107</v>
       </c>
@@ -887,7 +899,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>33</v>
       </c>
@@ -901,7 +913,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>34</v>
       </c>
@@ -915,7 +927,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>35</v>
       </c>
@@ -926,7 +938,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>36</v>
       </c>
@@ -937,7 +949,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>37</v>
       </c>
@@ -948,7 +960,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>39</v>
       </c>
@@ -959,22 +971,22 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="C13" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="C14" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="C15" s="2" t="s">
         <v>81</v>
       </c>
@@ -1333,7 +1345,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10AEA802-0E88-B24C-A9B4-36B13C3531BC}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
sync minigame to main game
</commit_message>
<xml_diff>
--- a/resources/gameBook.xlsx
+++ b/resources/gameBook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhhongxi/Desktop/LoversQuest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7212A80D-30AE-D942-9069-11D60EB637FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73585147-D64A-A845-9138-E5E7BDD9A146}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38380" yWindow="460" windowWidth="35840" windowHeight="20420" xr2:uid="{441C05F4-22D2-7348-A0BD-AC64BB4D47F4}"/>
+    <workbookView xWindow="1080" yWindow="540" windowWidth="35840" windowHeight="20420" activeTab="4" xr2:uid="{441C05F4-22D2-7348-A0BD-AC64BB4D47F4}"/>
   </bookViews>
   <sheets>
     <sheet name="objInGame" sheetId="7" r:id="rId1"/>
@@ -789,7 +789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51334EF7-C71C-3B45-98D3-0385A5E3D9BA}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -1192,7 +1192,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1461,8 +1461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF017B32-F13C-9940-ADCC-028F3D0515B4}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1524,7 +1524,7 @@
         <v>41</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D4" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
add highligher to key obj
</commit_message>
<xml_diff>
--- a/resources/gameBook.xlsx
+++ b/resources/gameBook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhhongxi/Desktop/LoversQuest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73585147-D64A-A845-9138-E5E7BDD9A146}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7992B854-04C4-8D4B-9E49-AE5D83F1EC83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="540" windowWidth="35840" windowHeight="20420" activeTab="4" xr2:uid="{441C05F4-22D2-7348-A0BD-AC64BB4D47F4}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20420" activeTab="2" xr2:uid="{441C05F4-22D2-7348-A0BD-AC64BB4D47F4}"/>
   </bookViews>
   <sheets>
     <sheet name="objInGame" sheetId="7" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="item" sheetId="3" r:id="rId3"/>
     <sheet name="container" sheetId="6" r:id="rId4"/>
     <sheet name="npc" sheetId="5" r:id="rId5"/>
+    <sheet name="miniGame" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="141">
   <si>
     <t xml:space="preserve">Name </t>
   </si>
@@ -205,9 +206,6 @@
     <t>portajohn</t>
   </si>
   <si>
-    <t>chowhall</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -256,12 +254,6 @@
     <t>You enjoy your soft shoe profile</t>
   </si>
   <si>
-    <t>Expert Marksmanship Badge</t>
-  </si>
-  <si>
-    <t>You can make things more deader better</t>
-  </si>
-  <si>
     <t>Combat Life Saver Badge</t>
   </si>
   <si>
@@ -331,9 +323,6 @@
     <t>M16 Assault Rifle, CamelBack,Sick call slip</t>
   </si>
   <si>
-    <t>Natural Lime WhiteClaw,Ruby Grapefruit WhiteClaw,Black Cherry WhiteClaw,Mango WhiteClaw,Diamond Ring</t>
-  </si>
-  <si>
     <t>ItemInContainer</t>
   </si>
   <si>
@@ -419,13 +408,64 @@
   </si>
   <si>
     <t>game</t>
+  </si>
+  <si>
+    <t>Safety Brief</t>
+  </si>
+  <si>
+    <t>PT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Range </t>
+  </si>
+  <si>
+    <t>Always point your rifle down range, click to shoot, if yo cannot shoot, you probably very good at doing details</t>
+  </si>
+  <si>
+    <t>CLS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Always wear your PT belt to stay safe, use your Racquet to hit the bouncing ball only! Don't use it on your battle buddies, if you fail the game, you will be voluntold to details   </t>
+  </si>
+  <si>
+    <t>You must find at least 70% right answer in order to pass the exam, if you fail the exam, you are going to do some "corrective training" with me</t>
+  </si>
+  <si>
+    <t>Army Marksmanship Expert Badge</t>
+  </si>
+  <si>
+    <t>Army Marksmanship Sharp Shooter Badge</t>
+  </si>
+  <si>
+    <t>Army Marksmanship Qualification Badge</t>
+  </si>
+  <si>
+    <t>you can make things more deader better than most jokers in your platoon</t>
+  </si>
+  <si>
+    <t>at least you hit a bit more than half targets at Range</t>
+  </si>
+  <si>
+    <t>you feel like your are the most lethal weapon of United State Army</t>
+  </si>
+  <si>
+    <t>chow hall</t>
+  </si>
+  <si>
+    <t>Natural Lime White Claw,Ruby Grapefruit White Claw,Black Cherry White Claw,Mango White Claw,Diamond Ring</t>
+  </si>
+  <si>
+    <t>It's size is twice as big as your pay check</t>
+  </si>
+  <si>
+    <t>diamond ring</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -446,6 +486,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -468,11 +514,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -787,208 +834,223 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51334EF7-C71C-3B45-98D3-0385A5E3D9BA}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="26.1640625" customWidth="1"/>
     <col min="2" max="2" width="25.5" customWidth="1"/>
-    <col min="3" max="3" width="28.5" customWidth="1"/>
+    <col min="3" max="3" width="44.33203125" customWidth="1"/>
     <col min="4" max="4" width="26.5" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" t="s">
         <v>117</v>
       </c>
-      <c r="E1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F1" t="s">
-        <v>121</v>
-      </c>
       <c r="G1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="19">
       <c r="A2" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="G2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="19">
       <c r="A3" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="19">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="19">
       <c r="A5" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="19">
       <c r="A6" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="19">
       <c r="A7" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="19">
       <c r="A8" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="19">
       <c r="A9" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="19">
       <c r="A10" s="3" t="s">
         <v>37</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="19">
       <c r="A11" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="19">
       <c r="C12" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="19">
       <c r="C13" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="19">
       <c r="C14" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="19">
       <c r="C15" s="2" t="s">
-        <v>81</v>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="18">
+      <c r="C16" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" ht="19">
+      <c r="C17" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" ht="19">
+      <c r="C18" s="2" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -1004,33 +1066,33 @@
       <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="5" width="14.5" customWidth="1"/>
     <col min="6" max="6" width="230.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="19">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="19">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1042,9 +1104,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="19">
       <c r="A3" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
@@ -1060,7 +1122,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="19">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1076,13 +1138,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="19">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>15</v>
@@ -1094,12 +1156,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="19">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -1108,7 +1170,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="19">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -1118,13 +1180,13 @@
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="19">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1138,7 +1200,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="19">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -1152,7 +1214,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="19">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -1168,7 +1230,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="19">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -1189,152 +1251,175 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2728922-B5F2-1D40-925B-F0E79ABFBC57}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="46.33203125" customWidth="1"/>
     <col min="2" max="2" width="38.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="19">
       <c r="A1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" ht="19">
+      <c r="A2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" ht="19">
+      <c r="A3" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" ht="19">
+      <c r="A4" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" ht="19">
+      <c r="A5" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" ht="19">
+      <c r="A6" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" ht="19">
+      <c r="A7" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" ht="19">
+      <c r="A8" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" ht="19">
+      <c r="A9" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" ht="19">
+      <c r="A10" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" ht="19">
+      <c r="A11" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" ht="19">
+      <c r="A12" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" ht="19">
+      <c r="A13" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C12" s="2"/>
-    </row>
-    <row r="13" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" ht="19">
+      <c r="A14" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="19">
       <c r="A15" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C15" s="2"/>
+        <v>131</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="19">
+      <c r="A16" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="19">
+      <c r="A17" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="19">
+      <c r="A18" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>139</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1346,10 +1431,10 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
     <col min="2" max="2" width="62.5" customWidth="1"/>
@@ -1357,96 +1442,96 @@
     <col min="4" max="4" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="19">
       <c r="A1" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="19">
       <c r="A2" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="19">
       <c r="A3" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="19">
       <c r="A4" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="19">
+      <c r="A5" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="19">
+      <c r="A6" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="B6" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="19">
       <c r="A7" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C7" t="s">
-        <v>98</v>
+        <v>138</v>
       </c>
       <c r="D7" t="s">
         <v>3</v>
@@ -1461,11 +1546,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF017B32-F13C-9940-ADCC-028F3D0515B4}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="27.1640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="62.33203125" style="3" customWidth="1"/>
@@ -1474,7 +1559,7 @@
     <col min="5" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1488,7 +1573,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
         <v>31</v>
       </c>
@@ -1502,7 +1587,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
         <v>32</v>
       </c>
@@ -1516,7 +1601,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1530,21 +1615,21 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="3" t="s">
         <v>33</v>
       </c>
@@ -1558,7 +1643,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" s="3" t="s">
         <v>34</v>
       </c>
@@ -1572,7 +1657,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" s="3" t="s">
         <v>35</v>
       </c>
@@ -1586,7 +1671,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" s="3" t="s">
         <v>36</v>
       </c>
@@ -1600,7 +1685,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" s="3" t="s">
         <v>37</v>
       </c>
@@ -1614,7 +1699,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11" s="3" t="s">
         <v>39</v>
       </c>
@@ -1622,10 +1707,58 @@
         <v>40</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>56</v>
+        <v>137</v>
       </c>
       <c r="D11" t="s">
         <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74728878-3D81-8E45-A835-A09EDB26C846}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="9.1640625" customWidth="1"/>
+    <col min="2" max="2" width="145" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="B1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add mini game together
</commit_message>
<xml_diff>
--- a/resources/gameBook.xlsx
+++ b/resources/gameBook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhhongxi/Desktop/LoversQuest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7992B854-04C4-8D4B-9E49-AE5D83F1EC83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F72B1DD-107D-874E-9FB5-7C18752F3FC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20420" activeTab="2" xr2:uid="{441C05F4-22D2-7348-A0BD-AC64BB4D47F4}"/>
+    <workbookView xWindow="38360" yWindow="500" windowWidth="35840" windowHeight="20420" xr2:uid="{441C05F4-22D2-7348-A0BD-AC64BB4D47F4}"/>
   </bookViews>
   <sheets>
     <sheet name="objInGame" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="142">
   <si>
     <t xml:space="preserve">Name </t>
   </si>
@@ -459,6 +459,9 @@
   </si>
   <si>
     <t>diamond ring</t>
+  </si>
+  <si>
+    <t>Drill SGT Tourniquet</t>
   </si>
 </sst>
 </file>
@@ -836,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51334EF7-C71C-3B45-98D3-0385A5E3D9BA}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -931,7 +934,7 @@
     </row>
     <row r="5" spans="1:7" ht="19">
       <c r="A5" s="3" t="s">
-        <v>103</v>
+        <v>141</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>85</v>
@@ -1253,7 +1256,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2728922-B5F2-1D40-925B-F0E79ABFBC57}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>

</xml_diff>